<commit_message>
UPDATE: Gamegrid, GameController. Tidsrapportering jimmy
</commit_message>
<xml_diff>
--- a/Documents/TimeReports/ProjectC4_TimeReport_Jimmy.xlsx
+++ b/Documents/TimeReports/ProjectC4_TimeReport_Jimmy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Översikt" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
   <si>
     <t>Tidrapport sammanfattning</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Grundstruktur i Android Studio. Finslip av dokumentation.</t>
+  </si>
+  <si>
+    <t>H-möte. Kodning av spellogik, vinst och lägga bricka.</t>
+  </si>
+  <si>
+    <t>Fungerande vinstkoll och optimering av spellogik.</t>
   </si>
 </sst>
 </file>
@@ -820,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -903,7 +909,7 @@
       </c>
       <c r="D10" s="17">
         <f>Mars!C42</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>4</v>
@@ -970,7 +976,7 @@
       </c>
       <c r="D16" s="19">
         <f>SUM(D10:D12)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>4</v>
@@ -992,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,7 +1071,7 @@
       </c>
       <c r="C8" s="28" t="str">
         <f>SUM(C11:C41) &amp; " h"</f>
-        <v>16 h</v>
+        <v>24 h</v>
       </c>
       <c r="D8" s="22"/>
     </row>
@@ -1265,15 +1271,23 @@
       <c r="B34" s="32">
         <v>42087</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="36"/>
+      <c r="C34" s="35">
+        <v>5</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="32">
         <v>42088</v>
       </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="36"/>
+      <c r="C35" s="35">
+        <v>3</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="32">
@@ -1323,7 +1337,7 @@
       </c>
       <c r="C42" s="40">
         <f>SUM(C11:C41)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D42" s="41" t="s">
         <v>13</v>

</xml_diff>